<commit_message>
fixed traj read real robot data
</commit_message>
<xml_diff>
--- a/my_package/traj_excel_10/tested_robot_traj_1_.xlsx
+++ b/my_package/traj_excel_10/tested_robot_traj_1_.xlsx
@@ -426,19 +426,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.2028864896758006</v>
+        <v>0.2028864896758006</v>
       </c>
       <c r="C1" t="n">
-        <v>1.56825683117444</v>
+        <v>0.002539495620456482</v>
       </c>
       <c r="D1" t="n">
-        <v>1.379316785363834</v>
+        <v>-1.379316785363834</v>
       </c>
       <c r="E1" t="n">
-        <v>1.381856437894394</v>
+        <v>0.188939888900502</v>
       </c>
       <c r="F1" t="n">
-        <v>-1.570796384046431</v>
+        <v>1.570796384046431</v>
       </c>
       <c r="G1" t="n">
         <v>-1.367909888287239</v>
@@ -449,19 +449,19 @@
         <v>0.221347107536837</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.2484977296296271</v>
+        <v>0.2484977296296271</v>
       </c>
       <c r="C2" t="n">
-        <v>1.568418617675491</v>
+        <v>0.002377709119405816</v>
       </c>
       <c r="D2" t="n">
-        <v>1.380518500463224</v>
+        <v>-1.380518500463224</v>
       </c>
       <c r="E2" t="n">
-        <v>1.382896364020461</v>
+        <v>0.1878999627744357</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.570796384423863</v>
+        <v>1.570796384423863</v>
       </c>
       <c r="G2" t="n">
         <v>-1.322298649847111</v>
@@ -472,19 +472,19 @@
         <v>0.4426942150736741</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.4528663241188721</v>
+        <v>0.4528663241188721</v>
       </c>
       <c r="C3" t="n">
-        <v>1.569143528461966</v>
+        <v>0.001652798332930176</v>
       </c>
       <c r="D3" t="n">
-        <v>1.385902980825687</v>
+        <v>-1.385902980825687</v>
       </c>
       <c r="E3" t="n">
-        <v>1.387555922519023</v>
+        <v>0.1832404042758736</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.570796386115009</v>
+        <v>1.570796386115009</v>
       </c>
       <c r="G3" t="n">
         <v>-1.117930062140237</v>
@@ -495,19 +495,19 @@
         <v>0.6640413226105111</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.7403935328885739</v>
+        <v>0.7403935328885739</v>
       </c>
       <c r="C4" t="n">
-        <v>1.570163409112236</v>
+        <v>0.0006329176826605036</v>
       </c>
       <c r="D4" t="n">
-        <v>1.393478433468806</v>
+        <v>-1.393478433468806</v>
       </c>
       <c r="E4" t="n">
-        <v>1.394111478926988</v>
+        <v>0.1766848478679089</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.570796388494291</v>
+        <v>1.570796388494291</v>
       </c>
       <c r="G4" t="n">
         <v>-0.8304028629126882</v>
@@ -518,19 +518,19 @@
         <v>0.8853884301473481</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.9447621273778194</v>
+        <v>0.9447621273778194</v>
       </c>
       <c r="C5" t="n">
-        <v>1.570888319898712</v>
+        <v>-9.199310381513776e-05</v>
       </c>
       <c r="D5" t="n">
-        <v>1.398862913831269</v>
+        <v>-1.398862913831269</v>
       </c>
       <c r="E5" t="n">
-        <v>1.39877103742555</v>
+        <v>0.1720252893693467</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.570796390185437</v>
+        <v>1.570796390185437</v>
       </c>
       <c r="G5" t="n">
         <v>-0.6260342752058142</v>
@@ -541,19 +541,19 @@
         <v>1.106735537684185</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.9903733673316449</v>
+        <v>0.9903733673316449</v>
       </c>
       <c r="C6" t="n">
-        <v>1.571050106399762</v>
+        <v>-0.0002537796048658041</v>
       </c>
       <c r="D6" t="n">
-        <v>1.40006462893066</v>
+        <v>-1.40006462893066</v>
       </c>
       <c r="E6" t="n">
-        <v>1.399810963551616</v>
+        <v>0.1709853632432805</v>
       </c>
       <c r="F6" t="n">
-        <v>-1.570796390562869</v>
+        <v>1.570796390562869</v>
       </c>
       <c r="G6" t="n">
         <v>-0.5804230367656862</v>

</xml_diff>